<commit_message>
changed back to old V3 ssoc assigner, GMI and HQA filtering was not helping
</commit_message>
<xml_diff>
--- a/output/CLFS_sample_input_validated.xlsx
+++ b/output/CLFS_sample_input_validated.xlsx
@@ -35,8 +35,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000000FF"/>
-        <bgColor rgb="000000FF"/>
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
       </patternFill>
     </fill>
     <fill>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:HP6"/>
+  <dimension ref="A1:HW6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -848,710 +848,745 @@
       </c>
       <c r="CE1" t="inlineStr">
         <is>
+          <t>SSIC Code</t>
+        </is>
+      </c>
+      <c r="CF1" t="inlineStr">
+        <is>
           <t>What were your reason(s) for being self-employed?</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>Would you prefer to be a/an</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>What were your reason(s) for taking up this job?</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>I was keen in this job and took it up because:</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>I was not keen in this job, but still took it up because:</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>Usual hours of work</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>FT/PT</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>Reason that working part time rather than full time?</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>The person you are mainly taking care of is your</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>What is his/her age?</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>Is he/she disabled/ill?</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>Main reason for working part-time rather than full-time:</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>Would you work full-time if suitable care services were available and/or affordable?</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>Willing to work additional hours?</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>Available for additional work?</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>Actively sought additional hours of work in the past four weeks?</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>GMI</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>Bonus received from your job(s) during the last 12 months</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>Employed for at least 10 months during the last 12 months?</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>How many jobs did you hold last week?</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>When did you begin working for your current employer?</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>Type of Employment?</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>Contract duration</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>Begin as a fixed-term contract employee in your current job?</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>Did your employer give you paid leave or compensation instead?</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>Did your employer give you paid sick leave when you were on MC</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>Did your employer give you at least one rest day each week?</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>Are you satisfied with your current job?</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>Are you actively looking for a new job?</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>How did you look for a job or employment during the last 4 weeks?</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>Are you looking for a permanent job?</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>Are you available to start work on the new job upon quitting the current job?</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DL1" t="inlineStr">
         <is>
           <t>Is the main reason for looking for a new job to better utilise your skills?</t>
         </is>
       </c>
-      <c r="DL1" t="inlineStr">
+      <c r="DM1" t="inlineStr">
         <is>
           <t>Number of Job changes in the last 2 years</t>
         </is>
       </c>
-      <c r="DM1" t="inlineStr">
+      <c r="DN1" t="inlineStr">
         <is>
           <t>When did you leave your last job?</t>
         </is>
       </c>
-      <c r="DN1" t="inlineStr">
+      <c r="DO1" t="inlineStr">
         <is>
           <t>Usual hours of work.1</t>
         </is>
       </c>
-      <c r="DO1" t="inlineStr">
+      <c r="DP1" t="inlineStr">
+        <is>
+          <t>FT/PT</t>
+        </is>
+      </c>
+      <c r="DQ1" t="inlineStr">
         <is>
           <t>Employment Status</t>
         </is>
       </c>
-      <c r="DP1" t="inlineStr">
+      <c r="DR1" t="inlineStr">
         <is>
           <t>Type of Employment?.1</t>
         </is>
       </c>
-      <c r="DQ1" t="inlineStr">
+      <c r="DS1" t="inlineStr">
         <is>
           <t>Contract duration.1</t>
         </is>
       </c>
-      <c r="DR1" t="inlineStr">
+      <c r="DT1" t="inlineStr">
         <is>
           <t>Job Title.1</t>
         </is>
       </c>
-      <c r="DS1" t="inlineStr">
+      <c r="DU1" t="inlineStr">
         <is>
           <t>Main tasks / duties.1</t>
         </is>
       </c>
-      <c r="DT1" t="inlineStr">
+      <c r="DV1" t="inlineStr">
+        <is>
+          <t>SSOC Code</t>
+        </is>
+      </c>
+      <c r="DW1" t="inlineStr">
         <is>
           <t>Name of Establishment you were working last worked</t>
         </is>
       </c>
-      <c r="DU1" t="inlineStr">
+      <c r="DX1" t="inlineStr">
         <is>
           <t>At what age did you start employment</t>
         </is>
       </c>
-      <c r="DV1" t="inlineStr">
+      <c r="DY1" t="inlineStr">
         <is>
           <t>Any breaks in employment?</t>
         </is>
       </c>
-      <c r="DW1" t="inlineStr">
+      <c r="DZ1" t="inlineStr">
         <is>
           <t>Ever relocated from Singapore to other countries for work?</t>
         </is>
       </c>
-      <c r="DX1" t="inlineStr">
+      <c r="EA1" t="inlineStr">
         <is>
           <t>When was your first such experience?</t>
         </is>
       </c>
-      <c r="DY1" t="inlineStr">
+      <c r="EB1" t="inlineStr">
         <is>
           <t>Total Duration</t>
         </is>
       </c>
-      <c r="DZ1" t="inlineStr">
+      <c r="EC1" t="inlineStr">
         <is>
           <t>How did that work stint arise?</t>
         </is>
       </c>
-      <c r="EA1" t="inlineStr">
+      <c r="ED1" t="inlineStr">
         <is>
           <t>Job title you worked in</t>
         </is>
       </c>
-      <c r="EB1" t="inlineStr">
+      <c r="EE1" t="inlineStr">
         <is>
           <t>Job industry or sector you worked in</t>
         </is>
       </c>
-      <c r="EC1" t="inlineStr">
+      <c r="EF1" t="inlineStr">
         <is>
           <t>Last drawn GMI</t>
         </is>
       </c>
-      <c r="ED1" t="inlineStr">
+      <c r="EG1" t="inlineStr">
         <is>
           <t>Company type</t>
         </is>
       </c>
-      <c r="EE1" t="inlineStr">
+      <c r="EH1" t="inlineStr">
         <is>
           <t>Location of work</t>
         </is>
       </c>
-      <c r="EF1" t="inlineStr">
+      <c r="EI1" t="inlineStr">
         <is>
           <t>Were you actively looking for jobs in the past 4 weeks?</t>
         </is>
       </c>
-      <c r="EG1" t="inlineStr">
+      <c r="EJ1" t="inlineStr">
         <is>
           <t>If no, what about at any point in time from 12 months ago till now?</t>
         </is>
       </c>
-      <c r="EH1" t="inlineStr">
+      <c r="EK1" t="inlineStr">
         <is>
           <t>At present, do you want to work?</t>
         </is>
       </c>
-      <c r="EI1" t="inlineStr">
+      <c r="EL1" t="inlineStr">
         <is>
           <t>Have you already secured a job?</t>
         </is>
       </c>
-      <c r="EJ1" t="inlineStr">
+      <c r="EM1" t="inlineStr">
         <is>
           <t>How soon do you expect to start working in this new job?</t>
         </is>
       </c>
-      <c r="EK1" t="inlineStr">
+      <c r="EN1" t="inlineStr">
         <is>
           <t>Are you available to work in the next 2 weeks?</t>
         </is>
       </c>
-      <c r="EL1" t="inlineStr">
+      <c r="EO1" t="inlineStr">
         <is>
           <t>When will you be available to work?</t>
         </is>
       </c>
-      <c r="EM1" t="inlineStr">
+      <c r="EP1" t="inlineStr">
         <is>
           <t>How long have you been looking for a job? (in weeks)</t>
         </is>
       </c>
-      <c r="EN1" t="inlineStr">
+      <c r="EQ1" t="inlineStr">
         <is>
           <t>While currently looking for work / waiting to start work, are you:</t>
         </is>
       </c>
-      <c r="EO1" t="inlineStr">
+      <c r="ER1" t="inlineStr">
         <is>
           <t>What kind of occupation were you looking for?</t>
         </is>
       </c>
-      <c r="EP1" t="inlineStr">
+      <c r="ES1" t="inlineStr">
         <is>
           <t>What was the main step you took to look for employment in the last 4 weeks?</t>
         </is>
       </c>
-      <c r="EQ1" t="inlineStr">
+      <c r="ET1" t="inlineStr">
         <is>
           <t>What other steps have you taken to look for employment in the last 4 weeks?</t>
         </is>
       </c>
-      <c r="ER1" t="inlineStr">
+      <c r="EU1" t="inlineStr">
         <is>
           <t>Did you experience difficulties while trying to secure a job?</t>
         </is>
       </c>
-      <c r="ES1" t="inlineStr">
+      <c r="EV1" t="inlineStr">
         <is>
           <t>Please indicate the main difficulty encountered:</t>
         </is>
       </c>
-      <c r="ET1" t="inlineStr">
+      <c r="EW1" t="inlineStr">
         <is>
           <t>What other difficulties did you encounter while trying to secure a job?</t>
         </is>
       </c>
-      <c r="EU1" t="inlineStr">
+      <c r="EX1" t="inlineStr">
         <is>
           <t>Have you ever worked before? (excluding full-time National Service)</t>
         </is>
       </c>
-      <c r="EV1" t="inlineStr">
+      <c r="EY1" t="inlineStr">
         <is>
           <t>Employment Status.1</t>
         </is>
       </c>
-      <c r="EW1" t="inlineStr">
+      <c r="EZ1" t="inlineStr">
         <is>
           <t>Job Title.2</t>
         </is>
       </c>
-      <c r="EX1" t="inlineStr">
+      <c r="FA1" t="inlineStr">
         <is>
           <t>Main tasks / duties.2</t>
         </is>
       </c>
-      <c r="EY1" t="inlineStr">
+      <c r="FB1" t="inlineStr">
+        <is>
+          <t>SSOC Code</t>
+        </is>
+      </c>
+      <c r="FC1" t="inlineStr">
         <is>
           <t>Name of Establishment you were working last worked.1</t>
         </is>
       </c>
-      <c r="EZ1" t="inlineStr">
+      <c r="FD1" t="inlineStr">
         <is>
           <t>Usual hours of work.2</t>
         </is>
       </c>
-      <c r="FA1" t="inlineStr">
+      <c r="FE1" t="inlineStr">
+        <is>
+          <t>FT/PT</t>
+        </is>
+      </c>
+      <c r="FF1" t="inlineStr">
         <is>
           <t>Last drawn GMI.1</t>
         </is>
       </c>
-      <c r="FB1" t="inlineStr">
+      <c r="FG1" t="inlineStr">
         <is>
           <t>What was the main reason you left your last job?</t>
         </is>
       </c>
-      <c r="FC1" t="inlineStr">
+      <c r="FH1" t="inlineStr">
         <is>
           <t>Please elaborate on the main reason for leaving your last job:</t>
         </is>
       </c>
-      <c r="FD1" t="inlineStr">
+      <c r="FI1" t="inlineStr">
         <is>
           <t>Please elaborate on the main reason for leaving your last job (Temporary in nature)</t>
         </is>
       </c>
-      <c r="FE1" t="inlineStr">
+      <c r="FJ1" t="inlineStr">
         <is>
           <t>Please elaborate on the main reason for leaving your last job (illness /Injury/accident)</t>
         </is>
       </c>
-      <c r="FF1" t="inlineStr">
+      <c r="FK1" t="inlineStr">
         <is>
           <t>The person you are mainly taking care of is your.1</t>
         </is>
       </c>
-      <c r="FG1" t="inlineStr">
+      <c r="FL1" t="inlineStr">
         <is>
           <t>What is his/her age?.1</t>
         </is>
       </c>
-      <c r="FH1" t="inlineStr">
+      <c r="FM1" t="inlineStr">
         <is>
           <t>Is he/she disabled/ill?.1</t>
         </is>
       </c>
-      <c r="FI1" t="inlineStr">
+      <c r="FN1" t="inlineStr">
         <is>
           <t>Main reason for leaving your last job due to care</t>
         </is>
       </c>
-      <c r="FJ1" t="inlineStr">
+      <c r="FO1" t="inlineStr">
         <is>
           <t>Would you work full-time if suitable care services were available and/or affordable?.1</t>
         </is>
       </c>
-      <c r="FK1" t="inlineStr">
+      <c r="FP1" t="inlineStr">
         <is>
           <t>When did you leave your last job? (In months)</t>
         </is>
       </c>
-      <c r="FL1" t="inlineStr">
+      <c r="FQ1" t="inlineStr">
         <is>
           <t>Ever relocated from Singapore to other countries for work?.1</t>
         </is>
       </c>
-      <c r="FM1" t="inlineStr">
+      <c r="FR1" t="inlineStr">
         <is>
           <t>When was your first such experience?.1</t>
         </is>
       </c>
-      <c r="FN1" t="inlineStr">
+      <c r="FS1" t="inlineStr">
         <is>
           <t>Total Duration.1</t>
         </is>
       </c>
-      <c r="FO1" t="inlineStr">
+      <c r="FT1" t="inlineStr">
         <is>
           <t>How did that work stint arise?.1</t>
         </is>
       </c>
-      <c r="FP1" t="inlineStr">
+      <c r="FU1" t="inlineStr">
         <is>
           <t>Job title you worked in.1</t>
         </is>
       </c>
-      <c r="FQ1" t="inlineStr">
+      <c r="FV1" t="inlineStr">
         <is>
           <t>Job industry or sector you worked in.1</t>
         </is>
       </c>
-      <c r="FR1" t="inlineStr">
+      <c r="FW1" t="inlineStr">
         <is>
           <t>Last drawn GMI.2</t>
         </is>
       </c>
-      <c r="FS1" t="inlineStr">
+      <c r="FX1" t="inlineStr">
         <is>
           <t>Company type.1</t>
         </is>
       </c>
-      <c r="FT1" t="inlineStr">
+      <c r="FY1" t="inlineStr">
         <is>
           <t>Location of work.1</t>
         </is>
       </c>
-      <c r="FU1" t="inlineStr">
+      <c r="FZ1" t="inlineStr">
         <is>
           <t>What is your main reason for not working and not looking for a job?</t>
         </is>
       </c>
-      <c r="FV1" t="inlineStr">
+      <c r="GA1" t="inlineStr">
         <is>
           <t>Have you ever retired from any job?.1</t>
         </is>
       </c>
-      <c r="FW1" t="inlineStr">
+      <c r="GB1" t="inlineStr">
         <is>
           <t>At what age retire?</t>
         </is>
       </c>
-      <c r="FX1" t="inlineStr">
+      <c r="GC1" t="inlineStr">
         <is>
           <t>The person you are mainly taking care of is your.2</t>
         </is>
       </c>
-      <c r="FY1" t="inlineStr">
+      <c r="GD1" t="inlineStr">
         <is>
           <t>What is his/her age?.2</t>
         </is>
       </c>
-      <c r="FZ1" t="inlineStr">
+      <c r="GE1" t="inlineStr">
         <is>
           <t>Is he/she disabled/ill?.2</t>
         </is>
       </c>
-      <c r="GA1" t="inlineStr">
+      <c r="GF1" t="inlineStr">
         <is>
           <t>Main reason for not working and not looking for job</t>
         </is>
       </c>
-      <c r="GB1" t="inlineStr">
+      <c r="GG1" t="inlineStr">
         <is>
           <t>Would you work if suitable care services were made available and/or affordable?</t>
         </is>
       </c>
-      <c r="GC1" t="inlineStr">
+      <c r="GH1" t="inlineStr">
         <is>
           <t>Have you ever worked before (excluding full-time National Service)?</t>
         </is>
       </c>
-      <c r="GD1" t="inlineStr">
+      <c r="GI1" t="inlineStr">
         <is>
           <t>When did you leave your last job? (Months)</t>
         </is>
       </c>
-      <c r="GE1" t="inlineStr">
+      <c r="GJ1" t="inlineStr">
         <is>
           <t>Employment Status.2</t>
         </is>
       </c>
-      <c r="GF1" t="inlineStr">
+      <c r="GK1" t="inlineStr">
         <is>
           <t>Job Title.3</t>
         </is>
       </c>
-      <c r="GG1" t="inlineStr">
+      <c r="GL1" t="inlineStr">
         <is>
           <t>Main tasks / duties.3</t>
         </is>
       </c>
-      <c r="GH1" t="inlineStr">
+      <c r="GM1" t="inlineStr">
+        <is>
+          <t>SSOC Code</t>
+        </is>
+      </c>
+      <c r="GN1" t="inlineStr">
         <is>
           <t>Name of Establishment you were working last worked.2</t>
         </is>
       </c>
-      <c r="GI1" t="inlineStr">
+      <c r="GO1" t="inlineStr">
         <is>
           <t>Usual hours of work.3</t>
         </is>
       </c>
-      <c r="GJ1" t="inlineStr">
+      <c r="GP1" t="inlineStr">
+        <is>
+          <t>FT/PT</t>
+        </is>
+      </c>
+      <c r="GQ1" t="inlineStr">
         <is>
           <t>Do you intend to look for a job in the future?</t>
         </is>
       </c>
-      <c r="GK1" t="inlineStr">
+      <c r="GR1" t="inlineStr">
         <is>
           <t>When do you intend to look for a job?</t>
         </is>
       </c>
-      <c r="GL1" t="inlineStr">
+      <c r="GS1" t="inlineStr">
         <is>
           <t>Do you prefer to work full-time or part-time?</t>
         </is>
       </c>
-      <c r="GM1" t="inlineStr">
+      <c r="GT1" t="inlineStr">
         <is>
           <t>At any point in the last 12 months, were you self-employed?</t>
         </is>
       </c>
-      <c r="GN1" t="inlineStr">
+      <c r="GU1" t="inlineStr">
         <is>
           <t>At any point in the last 12 months, were you self-employed?.1</t>
         </is>
       </c>
-      <c r="GO1" t="inlineStr">
+      <c r="GV1" t="inlineStr">
         <is>
           <t>At any point in the last 12 months, did you work on your own (i.e., without paid employees) while running your own business or trade?</t>
         </is>
       </c>
-      <c r="GP1" t="inlineStr">
+      <c r="GW1" t="inlineStr">
         <is>
           <t>Did you perform any freelance or assignment-based work via any of the following online platform(s) in the last 12 months?</t>
         </is>
       </c>
-      <c r="GQ1" t="inlineStr">
+      <c r="GX1" t="inlineStr">
         <is>
           <t>In the last 12 months, did you hold the following licence(s) or permits?</t>
         </is>
       </c>
-      <c r="GR1" t="inlineStr">
+      <c r="GY1" t="inlineStr">
         <is>
           <t>In the last 12 months, did you do any work related to the licence(s) held?</t>
         </is>
       </c>
-      <c r="GS1" t="inlineStr">
+      <c r="GZ1" t="inlineStr">
         <is>
           <t>Please indicate the main reason you were holding the licence(s) but not doing related work in the last 12 months?</t>
         </is>
       </c>
-      <c r="GT1" t="inlineStr">
+      <c r="HA1" t="inlineStr">
         <is>
           <t>How much interest did you receive from savings (e.g., current and saving accounts, fixed deposits) in the last 12 months?</t>
         </is>
       </c>
-      <c r="GU1" t="inlineStr">
+      <c r="HB1" t="inlineStr">
         <is>
           <t>Typically, savings accounts, current accounts or fixed deposits accrue interest, even for modest balances. For example, an account with $1,000 might earn $2 to $5 per year in interest. Considering this, would you like to revise your answer about interest earned?</t>
         </is>
       </c>
-      <c r="GV1" t="inlineStr">
+      <c r="HC1" t="inlineStr">
         <is>
           <t>Please indicate the amount you received from interest from savings in the last 12 months (e.g., current and saving accounts, fixed deposits)?</t>
         </is>
       </c>
-      <c r="GW1" t="inlineStr">
+      <c r="HD1" t="inlineStr">
         <is>
           <t>How much dividends and interests did you receive from other investment sources (e.g., bonds, shares, unit trust, personal loans to persons outside your households) in the last 12 months?</t>
         </is>
       </c>
-      <c r="GX1" t="inlineStr">
+      <c r="HE1" t="inlineStr">
         <is>
           <t>Did you receive any other income from non-employment sources e.g. from rental, social welfare grants in the last 12 months?</t>
         </is>
       </c>
-      <c r="GY1" t="inlineStr">
+      <c r="HF1" t="inlineStr">
         <is>
           <t>How much did you receive from rents (including rent from houses and fixed assets, subletting) in the last 12 months</t>
         </is>
       </c>
-      <c r="GZ1" t="inlineStr">
+      <c r="HG1" t="inlineStr">
         <is>
           <t>How much did you receive from regular cash and in-kind allowances or contributions (including alimony) from children, relatives, friends not staying in this household in the last 12 months</t>
         </is>
       </c>
-      <c r="HA1" t="inlineStr">
+      <c r="HH1" t="inlineStr">
         <is>
           <t>How much did you receive from sources other than employment and the above (e.g. regular pension payments, regular annuity payouts (excluding CPF Life, CPF Retirement Sum Scheme), social welfare grants, etc.) in the last 12 months</t>
         </is>
       </c>
-      <c r="HB1" t="inlineStr">
+      <c r="HI1" t="inlineStr">
         <is>
           <t>Do you provide care to any of the following individual(s) who is/are not fully independent and require(s) your assistance with their overall well-being (e.g. daily, medical, or developmental needs)?</t>
         </is>
       </c>
-      <c r="HC1" t="inlineStr">
+      <c r="HJ1" t="inlineStr">
         <is>
           <t>Do you provide care to any of the following individual(s) who is/are not fully independent and require(s) your assistance with their overall well-being (e.g. daily, medical, or developmental needs)?.1</t>
         </is>
       </c>
-      <c r="HD1" t="inlineStr">
+      <c r="HK1" t="inlineStr">
         <is>
           <t>Do any of these individual(s) have long-term care needs due to disability, illness, frailty, and/or mental health conditions?</t>
         </is>
       </c>
-      <c r="HE1" t="inlineStr">
+      <c r="HL1" t="inlineStr">
         <is>
           <t>The individual(s) with long term care needs whom you have been caring for is/are your</t>
         </is>
       </c>
-      <c r="HF1" t="inlineStr">
+      <c r="HM1" t="inlineStr">
         <is>
           <t>Relating to the individual(s) with long-term care needs due to disability, illness, frailty, and/or mental health conditions; how long have you been providing this caregiving support?</t>
         </is>
       </c>
-      <c r="HG1" t="inlineStr">
+      <c r="HN1" t="inlineStr">
         <is>
           <t>Do you expect to provide this caregiving support for at least 6 months?</t>
         </is>
       </c>
-      <c r="HH1" t="inlineStr">
+      <c r="HO1" t="inlineStr">
         <is>
           <t>Do you have difficulty seeing, even if wearing glasses?</t>
         </is>
       </c>
-      <c r="HI1" t="inlineStr">
+      <c r="HP1" t="inlineStr">
         <is>
           <t>Do you have difficulty hearing, even if using a hearing aid?</t>
         </is>
       </c>
-      <c r="HJ1" t="inlineStr">
+      <c r="HQ1" t="inlineStr">
         <is>
           <t>Do you have difficulty with body movement activities such as walking or climbing steps or transferring from bed to chair/wheelchair (and vice versa)?</t>
         </is>
       </c>
-      <c r="HK1" t="inlineStr">
+      <c r="HR1" t="inlineStr">
         <is>
           <t>Do you have difficulty with self-care activities such as washing all over (bath/shower) or dressing, feeding, or using the toilet?</t>
         </is>
       </c>
-      <c r="HL1" t="inlineStr">
+      <c r="HS1" t="inlineStr">
         <is>
           <t>Do you have the following long-lasting difficulties?</t>
         </is>
       </c>
-      <c r="HM1" t="inlineStr">
+      <c r="HT1" t="inlineStr">
         <is>
           <t>Does your current job accommodate the working arrangements you need (e.g. shorter working hours, provision of flexible work arrangements)?</t>
         </is>
       </c>
-      <c r="HN1" t="inlineStr">
+      <c r="HU1" t="inlineStr">
         <is>
           <t>Does your current job accommodate the working arrangements you need (e.g. shorter working hours, provision of flexible work arrangements)?.1</t>
         </is>
       </c>
-      <c r="HO1" t="inlineStr">
+      <c r="HV1" t="inlineStr">
         <is>
           <t>NS Industry</t>
         </is>
       </c>
-      <c r="HP1" t="inlineStr">
+      <c r="HW1" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
@@ -1753,6 +1788,11 @@
           <t>receives, stores and issues tools, merchandise, equipment or other goods and maintains relevant records</t>
         </is>
       </c>
+      <c r="BA2" s="1" t="inlineStr">
+        <is>
+          <t>43212</t>
+        </is>
+      </c>
       <c r="BB2" t="inlineStr">
         <is>
           <t>I have skills to carry out more complex tasks and duties</t>
@@ -1898,65 +1938,60 @@
           <t>Sheng Siong</t>
         </is>
       </c>
-      <c r="CG2" t="inlineStr">
+      <c r="CH2" t="inlineStr">
         <is>
           <t>I was keen in this job and took it up</t>
         </is>
       </c>
-      <c r="CH2" t="inlineStr">
+      <c r="CI2" t="inlineStr">
         <is>
           <t>The working hours suit me (i.e., the working time fits in well with my needs/activities);Of the flexibility in work schedule (i.e., possibility to adjust work schedule in response to work or personal needs)</t>
         </is>
       </c>
-      <c r="CJ2" t="n">
+      <c r="CK2" t="n">
         <v>30</v>
       </c>
-      <c r="CK2" s="1" t="inlineStr">
+      <c r="CL2" s="1" t="inlineStr">
         <is>
           <t>PT</t>
         </is>
       </c>
-      <c r="CL2" t="inlineStr">
+      <c r="CM2" t="inlineStr">
         <is>
           <t>Retired from full time employment</t>
         </is>
       </c>
-      <c r="CR2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="CU2" t="n">
+      <c r="CS2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CV2" t="n">
         <v>1900</v>
       </c>
-      <c r="CV2" t="n">
+      <c r="CW2" t="n">
         <v>0</v>
       </c>
-      <c r="CW2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
       <c r="CX2" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CY2" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="CY2" t="inlineStr">
+      <c r="CZ2" t="inlineStr">
         <is>
           <t>1 year ago</t>
         </is>
       </c>
-      <c r="CZ2" t="inlineStr">
+      <c r="DA2" t="inlineStr">
         <is>
           <t>Permanent Employee</t>
         </is>
       </c>
-      <c r="DB2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="DC2" t="inlineStr">
         <is>
           <t>No</t>
@@ -1969,7 +2004,7 @@
       </c>
       <c r="DE2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="DF2" t="inlineStr">
@@ -1979,88 +2014,93 @@
       </c>
       <c r="DG2" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="DL2" t="n">
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="DH2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="DM2" t="n">
         <v>0</v>
       </c>
-      <c r="GM2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GP2" t="inlineStr">
+      <c r="GT2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="GW2" t="inlineStr">
         <is>
           <t>I did not take up freelance or assignment-based work through online platforms in the last 12 months</t>
         </is>
       </c>
-      <c r="GQ2" t="inlineStr">
+      <c r="GX2" t="inlineStr">
         <is>
           <t>Private Hire Car Driver’s Vocational Licence (PDVL)</t>
         </is>
       </c>
-      <c r="GR2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GS2" t="inlineStr">
+      <c r="GY2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="GZ2" t="inlineStr">
         <is>
           <t>Obtained licence(s) as a backup plan</t>
         </is>
       </c>
-      <c r="GT2" t="n">
+      <c r="HA2" t="n">
         <v>5</v>
       </c>
-      <c r="GW2" t="n">
+      <c r="HD2" t="n">
         <v>0</v>
       </c>
-      <c r="GX2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="GY2" t="n">
+      <c r="HE2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="HF2" t="n">
         <v>2000</v>
       </c>
-      <c r="GZ2" t="n">
+      <c r="HG2" t="n">
         <v>500</v>
       </c>
-      <c r="HA2" t="n">
+      <c r="HH2" t="n">
         <v>600</v>
       </c>
-      <c r="HB2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="HH2" t="inlineStr">
+      <c r="HI2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HO2" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HI2" t="inlineStr">
+      <c r="HP2" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HJ2" t="inlineStr">
+      <c r="HQ2" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HK2" t="inlineStr">
+      <c r="HR2" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HL2" t="inlineStr">
+      <c r="HS2" t="inlineStr">
         <is>
           <t>None of the above</t>
         </is>
       </c>
-      <c r="HP2" t="inlineStr">
+      <c r="HW2" t="inlineStr">
         <is>
           <t>Husband living overseas currently</t>
         </is>
@@ -2154,9 +2194,9 @@
           <t>Residential unit</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>No religion;Christianity</t>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>No religion</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -2249,6 +2289,11 @@
           <t>manage a team of 30</t>
         </is>
       </c>
+      <c r="BA3" s="1" t="inlineStr">
+        <is>
+          <t>31004</t>
+        </is>
+      </c>
       <c r="BB3" t="inlineStr">
         <is>
           <t>My skills correspond to the skills needed</t>
@@ -2389,55 +2434,50 @@
           <t>singtel</t>
         </is>
       </c>
-      <c r="CG3" t="inlineStr">
+      <c r="CH3" t="inlineStr">
         <is>
           <t>I was keen in this job and took it up</t>
         </is>
       </c>
-      <c r="CH3" t="inlineStr">
+      <c r="CI3" t="inlineStr">
         <is>
           <t>Of the employee benefits (e.g., medical insurance)</t>
         </is>
       </c>
-      <c r="CJ3" t="n">
+      <c r="CK3" t="n">
         <v>60</v>
       </c>
-      <c r="CK3" s="1" t="inlineStr">
+      <c r="CL3" s="1" t="inlineStr">
         <is>
           <t>FT</t>
         </is>
       </c>
-      <c r="CU3" t="n">
+      <c r="CV3" t="n">
         <v>10000</v>
       </c>
-      <c r="CV3" t="n">
+      <c r="CW3" t="n">
         <v>1</v>
       </c>
-      <c r="CW3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="CX3" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CY3" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="CY3" t="inlineStr">
+      <c r="CZ3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="CZ3" t="inlineStr">
+      <c r="DA3" t="inlineStr">
         <is>
           <t>Permanent Employee</t>
         </is>
       </c>
-      <c r="DB3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="DC3" t="inlineStr">
         <is>
           <t>No</t>
@@ -2463,81 +2503,87 @@
           <t>No</t>
         </is>
       </c>
-      <c r="DL3" t="n">
+      <c r="DH3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="DM3" t="n">
         <v>0</v>
       </c>
-      <c r="GM3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GP3" s="2" t="inlineStr">
+      <c r="GT3" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="GV3" s="2" t="inlineStr"/>
+      <c r="GW3" s="2" t="inlineStr">
         <is>
           <t>Ride-hailing platforms (e.g. Grab Driver, GoPartner, Ryde Driver, TADA Driver)</t>
         </is>
       </c>
-      <c r="GQ3" t="inlineStr">
+      <c r="GX3" t="inlineStr">
         <is>
           <t>Taxi Driver’s Vocational Licence (TDVL)</t>
         </is>
       </c>
-      <c r="GR3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="GT3" s="2" t="n">
+      <c r="GY3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="HA3" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="GW3" t="n">
+      <c r="HD3" t="n">
         <v>0</v>
       </c>
-      <c r="GX3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="HB3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="HH3" t="inlineStr">
+      <c r="HE3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HI3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HO3" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HI3" t="inlineStr">
+      <c r="HP3" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HJ3" t="inlineStr">
+      <c r="HQ3" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HK3" t="inlineStr">
+      <c r="HR3" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HL3" t="inlineStr">
+      <c r="HS3" t="inlineStr">
         <is>
           <t>Visual impairment (Blindness or low vision that cannot be corrected)</t>
         </is>
       </c>
-      <c r="HM3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="HN3" t="inlineStr">
+      <c r="HT3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="HU3" t="inlineStr">
         <is>
           <t>Homeworking (Employees undertake work mainly in their homes without using information and communication technologies. Excludes those who are teleworking.)</t>
         </is>
       </c>
-      <c r="HP3" t="inlineStr">
+      <c r="HW3" t="inlineStr">
         <is>
           <t>respondent requests for dnc</t>
         </is>
@@ -2611,7 +2657,7 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="P4" s="1" t="inlineStr">
+      <c r="P4" s="2" t="inlineStr">
         <is>
           <t>Others: The RSPD confirms that the following answer is correct as of this time; United States of America</t>
         </is>
@@ -2641,12 +2687,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="CK4" s="1" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="HP4" t="inlineStr">
+      <c r="HW4" t="inlineStr">
         <is>
           <t>Can speak to my secretary Ms Karoline Leavitt for any queries, she can represent me , thank you,</t>
         </is>
@@ -2837,6 +2878,11 @@
           <t>development of mechatronic devices and applications through a combination of mechanical engineering. builds, tests, installs, and calibrates</t>
         </is>
       </c>
+      <c r="BA5" s="1" t="inlineStr">
+        <is>
+          <t>31291</t>
+        </is>
+      </c>
       <c r="BB5" t="inlineStr">
         <is>
           <t>My skills need to be further developed to cope with some of the tasks and duties</t>
@@ -2967,58 +3013,53 @@
           <t>daifuku mechatronic</t>
         </is>
       </c>
-      <c r="CG5" t="inlineStr">
+      <c r="CH5" t="inlineStr">
         <is>
           <t>I was not keen in this job, but still took it up</t>
         </is>
       </c>
-      <c r="CI5" t="inlineStr">
+      <c r="CJ5" t="inlineStr">
         <is>
           <t>There were no other job offers</t>
         </is>
       </c>
-      <c r="CJ5" t="n">
+      <c r="CK5" t="n">
         <v>44</v>
       </c>
-      <c r="CK5" s="1" t="inlineStr">
+      <c r="CL5" s="1" t="inlineStr">
         <is>
           <t>FT</t>
         </is>
       </c>
-      <c r="CU5" t="n">
+      <c r="CV5" t="n">
         <v>3800</v>
       </c>
-      <c r="CV5" t="n">
+      <c r="CW5" t="n">
         <v>1</v>
       </c>
-      <c r="CW5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="CX5" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CY5" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="CY5" t="inlineStr">
+      <c r="CZ5" t="inlineStr">
         <is>
           <t>6 months</t>
         </is>
       </c>
-      <c r="CZ5" s="2" t="inlineStr">
+      <c r="DA5" s="2" t="inlineStr">
         <is>
           <t>Permanent Employee</t>
         </is>
       </c>
-      <c r="DB5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="DC5" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="DD5" t="inlineStr">
@@ -3043,14 +3084,14 @@
       </c>
       <c r="DH5" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="DI5" t="inlineStr">
+        <is>
           <t>Placed or updated resumes on professional or social networking sites online (e.g. LinkedIn);Placed or answered online job advertisements</t>
         </is>
       </c>
-      <c r="DI5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
       <c r="DJ5" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -3058,133 +3099,143 @@
       </c>
       <c r="DK5" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="DL5" t="n">
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="DL5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="DM5" t="n">
         <v>2</v>
       </c>
-      <c r="DM5" t="inlineStr">
+      <c r="DN5" t="inlineStr">
         <is>
           <t>Less than 1 year ago</t>
         </is>
       </c>
-      <c r="DN5" t="n">
+      <c r="DO5" t="n">
         <v>30</v>
       </c>
-      <c r="DO5" t="inlineStr">
+      <c r="DP5" s="1" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="DQ5" t="inlineStr">
         <is>
           <t>Employee</t>
         </is>
       </c>
-      <c r="DP5" t="inlineStr">
+      <c r="DR5" t="inlineStr">
         <is>
           <t>Permanent Employee</t>
         </is>
       </c>
-      <c r="DR5" t="inlineStr">
+      <c r="DT5" t="inlineStr">
         <is>
           <t>Waitress</t>
         </is>
       </c>
-      <c r="DS5" t="inlineStr">
+      <c r="DU5" t="inlineStr">
         <is>
           <t>Serve food and beverages, handle cash transactions</t>
         </is>
       </c>
-      <c r="DT5" t="inlineStr">
+      <c r="DW5" t="inlineStr">
         <is>
           <t>Hai Di Lao</t>
         </is>
       </c>
-      <c r="DU5" t="n">
+      <c r="DX5" t="n">
         <v>21</v>
       </c>
-      <c r="DV5" t="n">
+      <c r="DY5" t="n">
         <v>3</v>
       </c>
-      <c r="DW5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GM5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="GN5" t="inlineStr">
+      <c r="DZ5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="GT5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="GU5" t="inlineStr">
         <is>
           <t>Running own business or trade</t>
         </is>
       </c>
-      <c r="GO5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="GP5" s="2" t="inlineStr">
+      <c r="GV5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="GW5" s="2" t="inlineStr">
         <is>
           <t>Food-delivery platforms (e.g. Deliveroo Rider, Foodpanda Rider, Grab Driver,</t>
         </is>
       </c>
-      <c r="GQ5" t="inlineStr">
+      <c r="GX5" t="inlineStr">
         <is>
           <t>None of the above</t>
         </is>
       </c>
-      <c r="GR5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GS5" t="inlineStr">
+      <c r="GY5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="GZ5" t="inlineStr">
         <is>
           <t>Obtained licence(s) as a backup plan</t>
         </is>
       </c>
-      <c r="GT5" t="n">
+      <c r="HA5" t="n">
         <v>10</v>
       </c>
-      <c r="GW5" t="n">
+      <c r="HD5" t="n">
         <v>0</v>
       </c>
-      <c r="GX5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="HB5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="HH5" t="inlineStr">
+      <c r="HE5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HI5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HO5" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HI5" t="inlineStr">
+      <c r="HP5" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HJ5" t="inlineStr">
+      <c r="HQ5" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HK5" t="inlineStr">
+      <c r="HR5" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HL5" t="inlineStr">
+      <c r="HS5" t="inlineStr">
         <is>
           <t>None of the above</t>
         </is>
       </c>
-      <c r="HP5" t="inlineStr">
+      <c r="HW5" t="inlineStr">
         <is>
           <t>nil</t>
         </is>
@@ -3258,7 +3309,7 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="P6" s="1" t="inlineStr">
+      <c r="P6" s="2" t="inlineStr">
         <is>
           <t>Others: The RSPD confirms that the following answer is correct as of this time; United States of America</t>
         </is>
@@ -3403,6 +3454,11 @@
           <t>Manage Country</t>
         </is>
       </c>
+      <c r="BA6" s="1" t="inlineStr">
+        <is>
+          <t>25233</t>
+        </is>
+      </c>
       <c r="BB6" t="inlineStr">
         <is>
           <t>My skills correspond to the skills needed</t>
@@ -3548,70 +3604,65 @@
           <t>White House</t>
         </is>
       </c>
-      <c r="CE6" t="inlineStr">
+      <c r="CF6" t="inlineStr">
         <is>
           <t>Control over my career</t>
         </is>
       </c>
-      <c r="CF6" t="inlineStr">
+      <c r="CG6" t="inlineStr">
         <is>
           <t>Self-employed</t>
         </is>
       </c>
-      <c r="CG6" t="inlineStr">
+      <c r="CH6" t="inlineStr">
         <is>
           <t>I was keen in this job and took it up</t>
         </is>
       </c>
-      <c r="CH6" t="inlineStr">
+      <c r="CI6" t="inlineStr">
         <is>
           <t>I find the work interesting/meaningful</t>
         </is>
       </c>
-      <c r="CJ6" t="n">
+      <c r="CK6" t="n">
         <v>50</v>
       </c>
-      <c r="CK6" s="1" t="inlineStr">
+      <c r="CL6" s="1" t="inlineStr">
         <is>
           <t>FT</t>
         </is>
       </c>
-      <c r="CU6" t="n">
+      <c r="CV6" t="n">
         <v>5000</v>
       </c>
-      <c r="CV6" t="n">
+      <c r="CW6" t="n">
         <v>0</v>
       </c>
-      <c r="CW6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
       <c r="CX6" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CY6" t="inlineStr">
+        <is>
           <t>3 or more</t>
         </is>
       </c>
-      <c r="CY6" t="inlineStr">
+      <c r="CZ6" t="inlineStr">
         <is>
           <t>1966</t>
         </is>
       </c>
-      <c r="CZ6" t="inlineStr">
+      <c r="DA6" t="inlineStr">
         <is>
           <t>Fixed-term Contract Employee</t>
         </is>
       </c>
-      <c r="DA6" t="inlineStr">
+      <c r="DB6" t="inlineStr">
         <is>
           <t>More than 1 - 2 years</t>
         </is>
       </c>
-      <c r="DC6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
       <c r="DD6" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -3634,109 +3685,114 @@
       </c>
       <c r="DH6" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="DI6" t="inlineStr">
+        <is>
           <t>Made preparations to start own business</t>
         </is>
       </c>
-      <c r="DI6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="DJ6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="DK6" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="DL6" t="n">
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="DL6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="DM6" t="n">
         <v>0</v>
       </c>
-      <c r="GM6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="GN6" t="inlineStr">
+      <c r="GT6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="GU6" t="inlineStr">
         <is>
           <t>Running own business or trade</t>
         </is>
       </c>
-      <c r="GO6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GP6" t="inlineStr">
+      <c r="GV6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="GW6" t="inlineStr">
         <is>
           <t>I did not take up freelance or assignment-based work through online platforms in the last 12 months</t>
         </is>
       </c>
-      <c r="GQ6" t="inlineStr">
+      <c r="GX6" t="inlineStr">
         <is>
           <t>None of the above</t>
         </is>
       </c>
-      <c r="GR6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GS6" t="inlineStr">
+      <c r="GY6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="GZ6" t="inlineStr">
         <is>
           <t>Obtained licence(s) as a backup plan</t>
         </is>
       </c>
-      <c r="GT6" t="n">
+      <c r="HA6" t="n">
         <v>0</v>
       </c>
-      <c r="GU6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="GW6" t="n">
+      <c r="HB6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HD6" t="n">
         <v>0</v>
       </c>
-      <c r="GX6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="HB6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="HH6" t="inlineStr">
+      <c r="HE6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HI6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="HO6" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HI6" t="inlineStr">
+      <c r="HP6" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HJ6" t="inlineStr">
+      <c r="HQ6" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HK6" t="inlineStr">
+      <c r="HR6" t="inlineStr">
         <is>
           <t>No – no difficulty</t>
         </is>
       </c>
-      <c r="HL6" t="inlineStr">
+      <c r="HS6" t="inlineStr">
         <is>
           <t>None of the above</t>
         </is>
       </c>
-      <c r="HP6" t="inlineStr">
+      <c r="HW6" t="inlineStr">
         <is>
           <t>Please contact my secretary Ms Karoline Leavitt if there are further queries.</t>
         </is>

</xml_diff>